<commit_message>
Reject appointment by interpreter is done.
</commit_message>
<xml_diff>
--- a/PLSI/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/PLSI/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashwini.G\eclipse-workspace\PLSI\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashwini.G\git\PLSI\PLSI\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA07A77-9388-4703-8159-236C7C7AAB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AAA0D7-46BE-4B60-8281-94B5811B009E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Description</t>
   </si>
@@ -43,22 +43,29 @@
   </si>
   <si>
     <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>Interpreter</t>
+  </si>
+  <si>
+    <t>wei.yuan@sstech.us</t>
+  </si>
+  <si>
+    <t>Invalid login</t>
+  </si>
+  <si>
+    <t>abc.sstech.us</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,6 +76,26 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,12 +120,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -383,58 +411,75 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.77734375" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.21875" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
+      <c r="B6" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{B0CAC26C-64D3-47B0-A768-D996A7769C2D}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{354A46C5-2038-40EF-BB36-5D12FB34A8FC}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{837E08DA-BF3A-4D21-8078-6314448C6B68}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{87BB022A-D23D-4BF8-AC9F-EBD381F53586}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Interpreter check in, check out,finalise,view finanacial details done
</commit_message>
<xml_diff>
--- a/PLSI/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/PLSI/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashwini.G\git\PLSI\PLSI\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AAA0D7-46BE-4B60-8281-94B5811B009E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF0DACF-1968-4295-ABE3-D61C11E25E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="New appointment" sheetId="3" r:id="rId2"/>
+    <sheet name="Reject app by Interpreter" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Description</t>
   </si>
@@ -58,6 +60,93 @@
   </si>
   <si>
     <t>xyz</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Appointment Date</t>
+  </si>
+  <si>
+    <t>App Start time</t>
+  </si>
+  <si>
+    <t>App End Time</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>App Type</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Patient Name</t>
+  </si>
+  <si>
+    <t>Requested Language</t>
+  </si>
+  <si>
+    <t>CHOP</t>
+  </si>
+  <si>
+    <t>CHOP Main</t>
+  </si>
+  <si>
+    <t>Fitness</t>
+  </si>
+  <si>
+    <t>Abramson Building</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Harsha</t>
+  </si>
+  <si>
+    <t>spanish</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Scheduler Username</t>
+  </si>
+  <si>
+    <t>Scheduler Password</t>
+  </si>
+  <si>
+    <t>Interpreter Username</t>
+  </si>
+  <si>
+    <t>Interpreter Password</t>
+  </si>
+  <si>
+    <t>Interpreter Name</t>
+  </si>
+  <si>
+    <t>Matt Laborde</t>
+  </si>
+  <si>
+    <t>matt.laborde@sstech.us</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>"16:15:00"</t>
+  </si>
+  <si>
+    <t>"16:35:00"</t>
+  </si>
+  <si>
+    <t>"23-12-2022"</t>
   </si>
 </sst>
 </file>
@@ -101,15 +190,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,16 +212,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -482,4 +596,181 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D46A24-3205-4CDB-80C0-67C7443BF381}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="12" max="12" width="19.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{8C2EDEAB-5424-4075-9274-B543BBAA5DA1}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{21395195-EBF5-4024-8E8E-9D6B3DD35A35}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABF68EE-3805-47F6-94A7-65083586E1E3}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="3" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{8DE6CF77-302C-4326-9EAE-3519D8EDFCBC}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{6FBA8F93-ABF4-456C-B097-2689B3FB54FD}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{74011E44-4203-4BC9-9098-395AA79CB576}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{4F79843C-FD5E-401F-8C70-1D1E8E702262}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data driven framework with interpreter reject,accept,checkin,chekout,finalise appointment.
</commit_message>
<xml_diff>
--- a/PLSI/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/PLSI/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashwini.G\git\PLSI\PLSI\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF0DACF-1968-4295-ABE3-D61C11E25E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CE7AFA-702B-4B00-BE2A-DF70662A5D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="New appointment" sheetId="3" r:id="rId2"/>
-    <sheet name="Reject app by Interpreter" sheetId="4" r:id="rId3"/>
+    <sheet name="Reject-Accept app" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Description</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>"23-12-2022"</t>
+  </si>
+  <si>
+    <t>Testname</t>
+  </si>
+  <si>
+    <t>Ashwini.</t>
   </si>
 </sst>
 </file>
@@ -600,10 +606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D46A24-3205-4CDB-80C0-67C7443BF381}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,7 +627,7 @@
     <col min="12" max="12" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -658,8 +664,11 @@
       <c r="L1" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -695,6 +704,9 @@
       </c>
       <c r="L2" t="s">
         <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -711,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABF68EE-3805-47F6-94A7-65083586E1E3}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>